<commit_message>
Update Relatorio-individual - Daniel.xlsx
</commit_message>
<xml_diff>
--- a/relatorios/Relatorio-individual - Daniel.xlsx
+++ b/relatorios/Relatorio-individual - Daniel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\vrumm\AINet\projetoAInet\relatorios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5397A8-6BEF-4960-86A6-F2D271898BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23957514-7E31-4351-AE3E-BB908220117B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="BDut9OBXirJHuaqMATYSYY0IcZ39UhQaxY4ivSAxhWFjLbwvdCvaNwz18ggAeakjbAy9PwMeCa+bzZHwGDmDUQ==" workbookSaltValue="6WTzD8wUpr5dqEHlS3NsMw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -728,8 +728,35 @@
       <alignment horizontal="right" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -746,33 +773,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1066,7 +1066,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
+      <selection pane="bottomLeft" activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21.95" customHeight="1"/>
@@ -1120,10 +1120,10 @@
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="36"/>
+      <c r="H4" s="44"/>
       <c r="I4" s="13"/>
       <c r="J4" s="21" t="s">
         <v>14</v>
@@ -1168,10 +1168,10 @@
       <c r="F6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="38"/>
+      <c r="H6" s="46"/>
       <c r="I6" s="18" t="s">
         <v>2</v>
       </c>
@@ -1201,10 +1201,10 @@
       <c r="F7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="37" t="s">
+      <c r="G7" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="38"/>
+      <c r="H7" s="46"/>
       <c r="I7" s="14"/>
       <c r="J7" s="22" t="s">
         <v>8</v>
@@ -1251,17 +1251,17 @@
       <c r="C11" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
       <c r="M11" s="14"/>
     </row>
     <row r="12" spans="1:13" ht="24" customHeight="1">
@@ -1269,17 +1269,17 @@
       <c r="C12" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
       <c r="M12" s="14"/>
     </row>
     <row r="13" spans="1:13" ht="24" customHeight="1">
@@ -1287,17 +1287,17 @@
       <c r="C13" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
       <c r="M13" s="14"/>
     </row>
     <row r="14" spans="1:13" ht="39" customHeight="1">
@@ -1305,17 +1305,17 @@
       <c r="C14" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
       <c r="M14" s="14"/>
     </row>
     <row r="15" spans="1:13" ht="39" customHeight="1">
@@ -1323,31 +1323,31 @@
       <c r="C15" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
       <c r="M15" s="14"/>
     </row>
     <row r="16" spans="1:13" ht="24" customHeight="1">
       <c r="B16" s="14"/>
       <c r="C16" s="27"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
       <c r="M16" s="14"/>
     </row>
     <row r="17" spans="2:13" ht="27" customHeight="1">
@@ -1355,12 +1355,12 @@
       <c r="C17" s="18"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="40" t="s">
+      <c r="F17" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
@@ -1374,11 +1374,11 @@
       <c r="F18" s="29">
         <v>0</v>
       </c>
-      <c r="G18" s="44" t="s">
+      <c r="G18" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
       <c r="J18" s="14"/>
       <c r="K18" s="14"/>
       <c r="L18" s="14"/>
@@ -1392,11 +1392,11 @@
       <c r="F19" s="29">
         <v>1</v>
       </c>
-      <c r="G19" s="44" t="s">
+      <c r="G19" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
       <c r="J19" s="14"/>
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
@@ -1410,11 +1410,11 @@
       <c r="F20" s="29">
         <v>2</v>
       </c>
-      <c r="G20" s="44" t="s">
+      <c r="G20" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
       <c r="J20" s="14"/>
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
@@ -1428,11 +1428,11 @@
       <c r="F21" s="29">
         <v>3</v>
       </c>
-      <c r="G21" s="44" t="s">
+      <c r="G21" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
       <c r="J21" s="14"/>
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
@@ -1442,39 +1442,39 @@
       <c r="F22" s="29">
         <v>4</v>
       </c>
-      <c r="G22" s="44" t="s">
+      <c r="G22" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="H22" s="44"/>
-      <c r="I22" s="44"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
     </row>
     <row r="23" spans="2:13" ht="18" customHeight="1">
       <c r="F23" s="25">
         <v>5</v>
       </c>
-      <c r="G23" s="44" t="s">
+      <c r="G23" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
     </row>
     <row r="24" spans="2:13" ht="9.9499999999999993" customHeight="1">
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="2:13" ht="36" customHeight="1">
-      <c r="B25" s="45" t="s">
+      <c r="B25" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="45"/>
-      <c r="L25" s="45"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
       <c r="M25" s="17"/>
     </row>
     <row r="26" spans="2:13" ht="29.1" customHeight="1">
@@ -1545,19 +1545,19 @@
     </row>
     <row r="29" spans="2:13" ht="14.1" customHeight="1"/>
     <row r="30" spans="2:13" ht="36" customHeight="1">
-      <c r="B30" s="46" t="s">
+      <c r="B30" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="46"/>
-      <c r="L30" s="46"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="41"/>
+      <c r="L30" s="41"/>
       <c r="M30" s="17"/>
     </row>
     <row r="31" spans="2:13" ht="36" customHeight="1">
@@ -1602,7 +1602,7 @@
         <v>47</v>
       </c>
       <c r="J32" s="23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K32" s="20">
         <v>3</v>
@@ -1741,19 +1741,19 @@
     <row r="39" spans="2:13" ht="14.1" customHeight="1"/>
     <row r="40" spans="2:13" ht="14.1" customHeight="1"/>
     <row r="41" spans="2:13" ht="36" customHeight="1">
-      <c r="B41" s="45" t="s">
+      <c r="B41" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="45"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
-      <c r="G41" s="45"/>
-      <c r="H41" s="45"/>
-      <c r="I41" s="45"/>
-      <c r="J41" s="45"/>
-      <c r="K41" s="45"/>
-      <c r="L41" s="45"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="40"/>
+      <c r="H41" s="40"/>
+      <c r="I41" s="40"/>
+      <c r="J41" s="40"/>
+      <c r="K41" s="40"/>
+      <c r="L41" s="40"/>
       <c r="M41" s="17"/>
     </row>
     <row r="42" spans="2:13" ht="21.95" customHeight="1">
@@ -1764,17 +1764,17 @@
       <c r="D42" s="7"/>
     </row>
     <row r="43" spans="2:13" ht="129.94999999999999" customHeight="1">
-      <c r="B43" s="41"/>
-      <c r="C43" s="42"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="42"/>
-      <c r="K43" s="42"/>
-      <c r="L43" s="43"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
+      <c r="K43" s="35"/>
+      <c r="L43" s="36"/>
       <c r="M43" s="32"/>
     </row>
     <row r="44" spans="2:13" ht="15" customHeight="1"/>
@@ -1788,6 +1788,21 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="onmbOWdCnm5cP1tCBX124PYJkRYa7UjJ5Wx31CPS7y5Sorj7U6RUhIX/UZQKXEhv4LqPYYwe5jo/WvFi7Jl8ZQ==" saltValue="KLxTWiXr2tx1ZWQvXTTT1Q==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="31">
+    <mergeCell ref="D13:L13"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="D12:L12"/>
+    <mergeCell ref="C36:H36"/>
+    <mergeCell ref="C37:H37"/>
+    <mergeCell ref="C38:H38"/>
+    <mergeCell ref="D14:L14"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="C34:H34"/>
+    <mergeCell ref="F17:I17"/>
     <mergeCell ref="B43:L43"/>
     <mergeCell ref="D11:L11"/>
     <mergeCell ref="D16:L16"/>
@@ -1804,21 +1819,6 @@
     <mergeCell ref="B25:L25"/>
     <mergeCell ref="G26:I26"/>
     <mergeCell ref="C35:H35"/>
-    <mergeCell ref="C36:H36"/>
-    <mergeCell ref="C37:H37"/>
-    <mergeCell ref="C38:H38"/>
-    <mergeCell ref="D14:L14"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="C32:H32"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="C34:H34"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="D13:L13"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="D12:L12"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="I31:L38">

</xml_diff>

<commit_message>
final commite - before vv rela
</commit_message>
<xml_diff>
--- a/relatorios/Relatorio-individual - Daniel.xlsx
+++ b/relatorios/Relatorio-individual - Daniel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\vrumm\AINet\projetoAInet\relatorios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23957514-7E31-4351-AE3E-BB908220117B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CD5106-13BF-4F07-8405-8305B67AD885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="BDut9OBXirJHuaqMATYSYY0IcZ39UhQaxY4ivSAxhWFjLbwvdCvaNwz18ggAeakjbAy9PwMeCa+bzZHwGDmDUQ==" workbookSaltValue="6WTzD8wUpr5dqEHlS3NsMw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -728,6 +728,31 @@
       <alignment horizontal="right" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
       <protection locked="0"/>
@@ -740,39 +765,14 @@
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1064,9 +1064,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DEBAC6A-54C1-F842-B37B-99052CD80123}">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J35" sqref="J35"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21.95" customHeight="1"/>
@@ -1120,10 +1120,10 @@
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="44"/>
+      <c r="H4" s="36"/>
       <c r="I4" s="13"/>
       <c r="J4" s="21" t="s">
         <v>14</v>
@@ -1168,10 +1168,10 @@
       <c r="F6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="45" t="s">
+      <c r="G6" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="46"/>
+      <c r="H6" s="38"/>
       <c r="I6" s="18" t="s">
         <v>2</v>
       </c>
@@ -1201,10 +1201,10 @@
       <c r="F7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="45" t="s">
+      <c r="G7" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="46"/>
+      <c r="H7" s="38"/>
       <c r="I7" s="14"/>
       <c r="J7" s="22" t="s">
         <v>8</v>
@@ -1251,17 +1251,17 @@
       <c r="C11" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="37"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
       <c r="M11" s="14"/>
     </row>
     <row r="12" spans="1:13" ht="24" customHeight="1">
@@ -1269,17 +1269,17 @@
       <c r="C12" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
       <c r="M12" s="14"/>
     </row>
     <row r="13" spans="1:13" ht="24" customHeight="1">
@@ -1287,17 +1287,17 @@
       <c r="C13" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="37"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
       <c r="M13" s="14"/>
     </row>
     <row r="14" spans="1:13" ht="39" customHeight="1">
@@ -1305,17 +1305,17 @@
       <c r="C14" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="37"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
       <c r="M14" s="14"/>
     </row>
     <row r="15" spans="1:13" ht="39" customHeight="1">
@@ -1323,31 +1323,31 @@
       <c r="C15" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
       <c r="M15" s="14"/>
     </row>
     <row r="16" spans="1:13" ht="24" customHeight="1">
       <c r="B16" s="14"/>
       <c r="C16" s="27"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
       <c r="M16" s="14"/>
     </row>
     <row r="17" spans="2:13" ht="27" customHeight="1">
@@ -1355,12 +1355,12 @@
       <c r="C17" s="18"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="42" t="s">
+      <c r="F17" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
@@ -1374,11 +1374,11 @@
       <c r="F18" s="29">
         <v>0</v>
       </c>
-      <c r="G18" s="38" t="s">
+      <c r="G18" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
       <c r="J18" s="14"/>
       <c r="K18" s="14"/>
       <c r="L18" s="14"/>
@@ -1392,11 +1392,11 @@
       <c r="F19" s="29">
         <v>1</v>
       </c>
-      <c r="G19" s="38" t="s">
+      <c r="G19" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
       <c r="J19" s="14"/>
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
@@ -1410,11 +1410,11 @@
       <c r="F20" s="29">
         <v>2</v>
       </c>
-      <c r="G20" s="38" t="s">
+      <c r="G20" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
       <c r="J20" s="14"/>
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
@@ -1428,11 +1428,11 @@
       <c r="F21" s="29">
         <v>3</v>
       </c>
-      <c r="G21" s="38" t="s">
+      <c r="G21" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
       <c r="J21" s="14"/>
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
@@ -1442,39 +1442,39 @@
       <c r="F22" s="29">
         <v>4</v>
       </c>
-      <c r="G22" s="38" t="s">
+      <c r="G22" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
     </row>
     <row r="23" spans="2:13" ht="18" customHeight="1">
       <c r="F23" s="25">
         <v>5</v>
       </c>
-      <c r="G23" s="38" t="s">
+      <c r="G23" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
     </row>
     <row r="24" spans="2:13" ht="9.9499999999999993" customHeight="1">
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="2:13" ht="36" customHeight="1">
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="45"/>
+      <c r="L25" s="45"/>
       <c r="M25" s="17"/>
     </row>
     <row r="26" spans="2:13" ht="29.1" customHeight="1">
@@ -1545,19 +1545,19 @@
     </row>
     <row r="29" spans="2:13" ht="14.1" customHeight="1"/>
     <row r="30" spans="2:13" ht="36" customHeight="1">
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="41"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="46"/>
       <c r="M30" s="17"/>
     </row>
     <row r="31" spans="2:13" ht="36" customHeight="1">
@@ -1608,7 +1608,7 @@
         <v>3</v>
       </c>
       <c r="L32" s="20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M32" s="32"/>
     </row>
@@ -1627,9 +1627,15 @@
       <c r="I33" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="J33" s="23"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
+      <c r="J33" s="23">
+        <v>3</v>
+      </c>
+      <c r="K33" s="20">
+        <v>2</v>
+      </c>
+      <c r="L33" s="20">
+        <v>2</v>
+      </c>
       <c r="M33" s="32"/>
     </row>
     <row r="34" spans="2:13" ht="36" customHeight="1">
@@ -1667,9 +1673,15 @@
       <c r="I35" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="J35" s="23"/>
-      <c r="K35" s="20"/>
-      <c r="L35" s="20"/>
+      <c r="J35" s="23">
+        <v>3</v>
+      </c>
+      <c r="K35" s="20">
+        <v>2</v>
+      </c>
+      <c r="L35" s="20">
+        <v>3</v>
+      </c>
       <c r="M35" s="32"/>
     </row>
     <row r="36" spans="2:13" ht="36" customHeight="1">
@@ -1741,19 +1753,19 @@
     <row r="39" spans="2:13" ht="14.1" customHeight="1"/>
     <row r="40" spans="2:13" ht="14.1" customHeight="1"/>
     <row r="41" spans="2:13" ht="36" customHeight="1">
-      <c r="B41" s="40" t="s">
+      <c r="B41" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="40"/>
-      <c r="D41" s="40"/>
-      <c r="E41" s="40"/>
-      <c r="F41" s="40"/>
-      <c r="G41" s="40"/>
-      <c r="H41" s="40"/>
-      <c r="I41" s="40"/>
-      <c r="J41" s="40"/>
-      <c r="K41" s="40"/>
-      <c r="L41" s="40"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="45"/>
+      <c r="J41" s="45"/>
+      <c r="K41" s="45"/>
+      <c r="L41" s="45"/>
       <c r="M41" s="17"/>
     </row>
     <row r="42" spans="2:13" ht="21.95" customHeight="1">
@@ -1764,17 +1776,17 @@
       <c r="D42" s="7"/>
     </row>
     <row r="43" spans="2:13" ht="129.94999999999999" customHeight="1">
-      <c r="B43" s="34"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
-      <c r="K43" s="35"/>
-      <c r="L43" s="36"/>
+      <c r="B43" s="41"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
+      <c r="K43" s="42"/>
+      <c r="L43" s="43"/>
       <c r="M43" s="32"/>
     </row>
     <row r="44" spans="2:13" ht="15" customHeight="1"/>
@@ -1788,21 +1800,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="onmbOWdCnm5cP1tCBX124PYJkRYa7UjJ5Wx31CPS7y5Sorj7U6RUhIX/UZQKXEhv4LqPYYwe5jo/WvFi7Jl8ZQ==" saltValue="KLxTWiXr2tx1ZWQvXTTT1Q==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="31">
-    <mergeCell ref="D13:L13"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="D12:L12"/>
-    <mergeCell ref="C36:H36"/>
-    <mergeCell ref="C37:H37"/>
-    <mergeCell ref="C38:H38"/>
-    <mergeCell ref="D14:L14"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="C32:H32"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="C34:H34"/>
-    <mergeCell ref="F17:I17"/>
     <mergeCell ref="B43:L43"/>
     <mergeCell ref="D11:L11"/>
     <mergeCell ref="D16:L16"/>
@@ -1819,6 +1816,21 @@
     <mergeCell ref="B25:L25"/>
     <mergeCell ref="G26:I26"/>
     <mergeCell ref="C35:H35"/>
+    <mergeCell ref="C36:H36"/>
+    <mergeCell ref="C37:H37"/>
+    <mergeCell ref="C38:H38"/>
+    <mergeCell ref="D14:L14"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="C34:H34"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="D13:L13"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="D12:L12"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="I31:L38">

</xml_diff>